<commit_message>
Updated tests for Robot Meta Tag and updated the dataprovider
</commit_message>
<xml_diff>
--- a/test-data/page-with-metatag-data.xlsx
+++ b/test-data/page-with-metatag-data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8DCB15-7087-4C0A-81F9-50E30BBB6539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E9D360-707F-456D-A52A-E1E61044DD03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>path</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>/about-cancer/causes-prevention/vitamin-d-fact-sheet</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/self-image</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD1206-3591-4D75-B37B-F40530826E59}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +482,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>